<commit_message>
append xy coordinate to the dataset filtered
</commit_message>
<xml_diff>
--- a/gis/sand/砂层.xlsx
+++ b/gis/sand/砂层.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R234"/>
+  <dimension ref="A1:T234"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,10 +512,20 @@
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
+          <t>X坐标</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Y坐标</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>实际层顶埋深</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>实际层底埋深</t>
         </is>
@@ -573,9 +583,15 @@
         <v>2.3</v>
       </c>
       <c r="Q2" t="n">
+        <v>3396.6102</v>
+      </c>
+      <c r="R2" t="n">
+        <v>1350.98811893196</v>
+      </c>
+      <c r="S2" t="n">
         <v>-16.7</v>
       </c>
-      <c r="R2" t="n">
+      <c r="T2" t="n">
         <v>-31.7</v>
       </c>
     </row>
@@ -631,9 +647,15 @@
         <v>3.53</v>
       </c>
       <c r="Q3" t="n">
+        <v>4727.49120000002</v>
+      </c>
+      <c r="R3" t="n">
+        <v>2028.39078559882</v>
+      </c>
+      <c r="S3" t="n">
         <v>-23.47</v>
       </c>
-      <c r="R3" t="n">
+      <c r="T3" t="n">
         <v>-30.87</v>
       </c>
     </row>
@@ -689,9 +711,15 @@
         <v>3.53</v>
       </c>
       <c r="Q4" t="n">
+        <v>4727.49120000002</v>
+      </c>
+      <c r="R4" t="n">
+        <v>2028.39078559882</v>
+      </c>
+      <c r="S4" t="n">
         <v>-30.87</v>
       </c>
-      <c r="R4" t="n">
+      <c r="T4" t="n">
         <v>-37.27</v>
       </c>
     </row>
@@ -747,9 +775,15 @@
         <v>3.92</v>
       </c>
       <c r="Q5" t="n">
+        <v>2984.6562</v>
+      </c>
+      <c r="R5" t="n">
+        <v>3769.98411893224</v>
+      </c>
+      <c r="S5" t="n">
         <v>-30.18</v>
       </c>
-      <c r="R5" t="n">
+      <c r="T5" t="n">
         <v>-39.18</v>
       </c>
     </row>
@@ -805,9 +839,15 @@
         <v>-2.69</v>
       </c>
       <c r="Q6" t="n">
+        <v>8381.317045500011</v>
+      </c>
+      <c r="R6" t="n">
+        <v>-1256.70173906783</v>
+      </c>
+      <c r="S6" t="n">
         <v>-26.49</v>
       </c>
-      <c r="R6" t="n">
+      <c r="T6" t="n">
         <v>-28.49</v>
       </c>
     </row>
@@ -863,9 +903,15 @@
         <v>-2.69</v>
       </c>
       <c r="Q7" t="n">
+        <v>8381.317045500011</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-1256.70173906783</v>
+      </c>
+      <c r="S7" t="n">
         <v>-28.99</v>
       </c>
-      <c r="R7" t="n">
+      <c r="T7" t="n">
         <v>-30.29</v>
       </c>
     </row>
@@ -921,9 +967,15 @@
         <v>-0.85</v>
       </c>
       <c r="Q8" t="n">
+        <v>2898.48982200006</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-5027.45854840117</v>
+      </c>
+      <c r="S8" t="n">
         <v>-26.25</v>
       </c>
-      <c r="R8" t="n">
+      <c r="T8" t="n">
         <v>-29.45</v>
       </c>
     </row>
@@ -979,9 +1031,15 @@
         <v>-0.79</v>
       </c>
       <c r="Q9" t="n">
+        <v>7013.33014650005</v>
+      </c>
+      <c r="R9" t="n">
+        <v>3245.5615229321</v>
+      </c>
+      <c r="S9" t="n">
         <v>-20.09</v>
       </c>
-      <c r="R9" t="n">
+      <c r="T9" t="n">
         <v>-20.79</v>
       </c>
     </row>
@@ -1037,9 +1095,15 @@
         <v>-0.79</v>
       </c>
       <c r="Q10" t="n">
+        <v>7013.33014650005</v>
+      </c>
+      <c r="R10" t="n">
+        <v>3245.5615229321</v>
+      </c>
+      <c r="S10" t="n">
         <v>-20.79</v>
       </c>
-      <c r="R10" t="n">
+      <c r="T10" t="n">
         <v>-30.19</v>
       </c>
     </row>
@@ -1095,9 +1159,15 @@
         <v>-0.79</v>
       </c>
       <c r="Q11" t="n">
+        <v>7013.33014650005</v>
+      </c>
+      <c r="R11" t="n">
+        <v>3245.5615229321</v>
+      </c>
+      <c r="S11" t="n">
         <v>-35.49</v>
       </c>
-      <c r="R11" t="n">
+      <c r="T11" t="n">
         <v>-39.19</v>
       </c>
     </row>
@@ -1153,9 +1223,15 @@
         <v>-3.85</v>
       </c>
       <c r="Q12" t="n">
+        <v>8277.53302650005</v>
+      </c>
+      <c r="R12" t="n">
+        <v>1523.38387093196</v>
+      </c>
+      <c r="S12" t="n">
         <v>-39.05</v>
       </c>
-      <c r="R12" t="n">
+      <c r="T12" t="n">
         <v>-41.45</v>
       </c>
     </row>
@@ -1211,9 +1287,15 @@
         <v>-3.85</v>
       </c>
       <c r="Q13" t="n">
+        <v>8277.53302650005</v>
+      </c>
+      <c r="R13" t="n">
+        <v>1523.38387093196</v>
+      </c>
+      <c r="S13" t="n">
         <v>-41.45</v>
       </c>
-      <c r="R13" t="n">
+      <c r="T13" t="n">
         <v>-43.85</v>
       </c>
     </row>
@@ -1269,9 +1351,15 @@
         <v>-0.52</v>
       </c>
       <c r="Q14" t="n">
+        <v>7029.03060600001</v>
+      </c>
+      <c r="R14" t="n">
+        <v>2387.92326026534</v>
+      </c>
+      <c r="S14" t="n">
         <v>-25.12</v>
       </c>
-      <c r="R14" t="n">
+      <c r="T14" t="n">
         <v>-30.22</v>
       </c>
     </row>
@@ -1327,9 +1415,15 @@
         <v>-0.52</v>
       </c>
       <c r="Q15" t="n">
+        <v>7029.03060600001</v>
+      </c>
+      <c r="R15" t="n">
+        <v>2387.92326026534</v>
+      </c>
+      <c r="S15" t="n">
         <v>-32.82</v>
       </c>
-      <c r="R15" t="n">
+      <c r="T15" t="n">
         <v>-41.02</v>
       </c>
     </row>
@@ -1385,9 +1479,15 @@
         <v>-0.27</v>
       </c>
       <c r="Q16" t="n">
+        <v>4821.45804600004</v>
+      </c>
+      <c r="R16" t="n">
+        <v>-2236.63373840135</v>
+      </c>
+      <c r="S16" t="n">
         <v>-24.27</v>
       </c>
-      <c r="R16" t="n">
+      <c r="T16" t="n">
         <v>-27.27</v>
       </c>
     </row>
@@ -1443,9 +1543,15 @@
         <v>-0.27</v>
       </c>
       <c r="Q17" t="n">
+        <v>4821.45804600004</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-2236.63373840135</v>
+      </c>
+      <c r="S17" t="n">
         <v>-27.27</v>
       </c>
-      <c r="R17" t="n">
+      <c r="T17" t="n">
         <v>-30.67</v>
       </c>
     </row>
@@ -1501,9 +1607,15 @@
         <v>-0.39</v>
       </c>
       <c r="Q18" t="n">
+        <v>1884.17438850005</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-2497.48408906783</v>
+      </c>
+      <c r="S18" t="n">
         <v>-28.19</v>
       </c>
-      <c r="R18" t="n">
+      <c r="T18" t="n">
         <v>-29.99</v>
       </c>
     </row>
@@ -1555,9 +1667,15 @@
         <v>-0.17</v>
       </c>
       <c r="Q19" t="n">
+        <v>2178.231222</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-3148.1280724012</v>
+      </c>
+      <c r="S19" t="n">
         <v>-15.17</v>
       </c>
-      <c r="R19" t="n">
+      <c r="T19" t="n">
         <v>-15.87</v>
       </c>
     </row>
@@ -1609,9 +1727,15 @@
         <v>-0.17</v>
       </c>
       <c r="Q20" t="n">
+        <v>2178.231222</v>
+      </c>
+      <c r="R20" t="n">
+        <v>-3148.1280724012</v>
+      </c>
+      <c r="S20" t="n">
         <v>-22.37</v>
       </c>
-      <c r="R20" t="n">
+      <c r="T20" t="n">
         <v>-24.17</v>
       </c>
     </row>
@@ -1663,9 +1787,15 @@
         <v>-0.17</v>
       </c>
       <c r="Q21" t="n">
+        <v>2178.231222</v>
+      </c>
+      <c r="R21" t="n">
+        <v>-3148.1280724012</v>
+      </c>
+      <c r="S21" t="n">
         <v>-24.17</v>
       </c>
-      <c r="R21" t="n">
+      <c r="T21" t="n">
         <v>-26.67</v>
       </c>
     </row>
@@ -1717,9 +1847,15 @@
         <v>-0.53</v>
       </c>
       <c r="Q22" t="n">
+        <v>2334.66967800001</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-3795.73174440116</v>
+      </c>
+      <c r="S22" t="n">
         <v>-18.93</v>
       </c>
-      <c r="R22" t="n">
+      <c r="T22" t="n">
         <v>-20.93</v>
       </c>
     </row>
@@ -1771,9 +1907,15 @@
         <v>-0.53</v>
       </c>
       <c r="Q23" t="n">
+        <v>2334.66967800001</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-3795.73174440116</v>
+      </c>
+      <c r="S23" t="n">
         <v>-20.93</v>
       </c>
-      <c r="R23" t="n">
+      <c r="T23" t="n">
         <v>-23.03</v>
       </c>
     </row>
@@ -1825,9 +1967,15 @@
         <v>0.09</v>
       </c>
       <c r="Q24" t="n">
+        <v>2979.11156699999</v>
+      </c>
+      <c r="R24" t="n">
+        <v>-1694.09639640121</v>
+      </c>
+      <c r="S24" t="n">
         <v>-26.21</v>
       </c>
-      <c r="R24" t="n">
+      <c r="T24" t="n">
         <v>-27.01</v>
       </c>
     </row>
@@ -1879,9 +2027,15 @@
         <v>-0.2</v>
       </c>
       <c r="Q25" t="n">
+        <v>3189.57018450001</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-2347.50558040136</v>
+      </c>
+      <c r="S25" t="n">
         <v>-16.2</v>
       </c>
-      <c r="R25" t="n">
+      <c r="T25" t="n">
         <v>-18.6</v>
       </c>
     </row>
@@ -1933,9 +2087,15 @@
         <v>-0.89</v>
       </c>
       <c r="Q26" t="n">
+        <v>3580.13928300006</v>
+      </c>
+      <c r="R26" t="n">
+        <v>-3007.48423106782</v>
+      </c>
+      <c r="S26" t="n">
         <v>-20.49</v>
       </c>
-      <c r="R26" t="n">
+      <c r="T26" t="n">
         <v>-24.39</v>
       </c>
     </row>
@@ -1987,9 +2147,15 @@
         <v>-0.1</v>
       </c>
       <c r="Q27" t="n">
+        <v>3881.50878300006</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-3674.53058573448</v>
+      </c>
+      <c r="S27" t="n">
         <v>-15.4</v>
       </c>
-      <c r="R27" t="n">
+      <c r="T27" t="n">
         <v>-18.1</v>
       </c>
     </row>
@@ -2041,9 +2207,15 @@
         <v>-0.1</v>
       </c>
       <c r="Q28" t="n">
+        <v>3881.50878300006</v>
+      </c>
+      <c r="R28" t="n">
+        <v>-3674.53058573448</v>
+      </c>
+      <c r="S28" t="n">
         <v>-18.1</v>
       </c>
-      <c r="R28" t="n">
+      <c r="T28" t="n">
         <v>-21.1</v>
       </c>
     </row>
@@ -2095,9 +2267,15 @@
         <v>-0.1</v>
       </c>
       <c r="Q29" t="n">
+        <v>3881.50878300006</v>
+      </c>
+      <c r="R29" t="n">
+        <v>-3674.53058573448</v>
+      </c>
+      <c r="S29" t="n">
         <v>-21.1</v>
       </c>
-      <c r="R29" t="n">
+      <c r="T29" t="n">
         <v>-25.1</v>
       </c>
     </row>
@@ -2149,9 +2327,15 @@
         <v>0.2</v>
       </c>
       <c r="Q30" t="n">
+        <v>4188.21159300001</v>
+      </c>
+      <c r="R30" t="n">
+        <v>-4316.15174106788</v>
+      </c>
+      <c r="S30" t="n">
         <v>-17.5</v>
       </c>
-      <c r="R30" t="n">
+      <c r="T30" t="n">
         <v>-18.1</v>
       </c>
     </row>
@@ -2203,9 +2387,15 @@
         <v>0.2</v>
       </c>
       <c r="Q31" t="n">
+        <v>4188.21159300001</v>
+      </c>
+      <c r="R31" t="n">
+        <v>-4316.15174106788</v>
+      </c>
+      <c r="S31" t="n">
         <v>-18.1</v>
       </c>
-      <c r="R31" t="n">
+      <c r="T31" t="n">
         <v>-20.1</v>
       </c>
     </row>
@@ -2257,9 +2447,15 @@
         <v>0.2</v>
       </c>
       <c r="Q32" t="n">
+        <v>4188.21159300001</v>
+      </c>
+      <c r="R32" t="n">
+        <v>-4316.15174106788</v>
+      </c>
+      <c r="S32" t="n">
         <v>-24.6</v>
       </c>
-      <c r="R32" t="n">
+      <c r="T32" t="n">
         <v>-26</v>
       </c>
     </row>
@@ -2315,9 +2511,15 @@
         <v>0.12</v>
       </c>
       <c r="Q33" t="n">
+        <v>4504.27606800006</v>
+      </c>
+      <c r="R33" t="n">
+        <v>-1557.67802373444</v>
+      </c>
+      <c r="S33" t="n">
         <v>-20.78</v>
       </c>
-      <c r="R33" t="n">
+      <c r="T33" t="n">
         <v>-21.68</v>
       </c>
     </row>
@@ -2373,9 +2575,15 @@
         <v>0.12</v>
       </c>
       <c r="Q34" t="n">
+        <v>4504.27606800006</v>
+      </c>
+      <c r="R34" t="n">
+        <v>-1557.67802373444</v>
+      </c>
+      <c r="S34" t="n">
         <v>-21.68</v>
       </c>
-      <c r="R34" t="n">
+      <c r="T34" t="n">
         <v>-22.48</v>
       </c>
     </row>
@@ -2431,9 +2639,15 @@
         <v>0.08</v>
       </c>
       <c r="Q35" t="n">
+        <v>5130.74679450004</v>
+      </c>
+      <c r="R35" t="n">
+        <v>-2878.86874040123</v>
+      </c>
+      <c r="S35" t="n">
         <v>-24.22</v>
       </c>
-      <c r="R35" t="n">
+      <c r="T35" t="n">
         <v>-24.92</v>
       </c>
     </row>
@@ -2489,9 +2703,15 @@
         <v>-0.09</v>
       </c>
       <c r="Q36" t="n">
+        <v>5562.78148200005</v>
+      </c>
+      <c r="R36" t="n">
+        <v>-4177.88312973455</v>
+      </c>
+      <c r="S36" t="n">
         <v>-23.59</v>
       </c>
-      <c r="R36" t="n">
+      <c r="T36" t="n">
         <v>-26.09</v>
       </c>
     </row>
@@ -2547,9 +2767,15 @@
         <v>-0.09</v>
       </c>
       <c r="Q37" t="n">
+        <v>5562.78148200005</v>
+      </c>
+      <c r="R37" t="n">
+        <v>-4177.88312973455</v>
+      </c>
+      <c r="S37" t="n">
         <v>-26.09</v>
       </c>
-      <c r="R37" t="n">
+      <c r="T37" t="n">
         <v>-29.09</v>
       </c>
     </row>
@@ -2605,9 +2831,15 @@
         <v>-0.09</v>
       </c>
       <c r="Q38" t="n">
+        <v>5562.78148200005</v>
+      </c>
+      <c r="R38" t="n">
+        <v>-4177.88312973455</v>
+      </c>
+      <c r="S38" t="n">
         <v>-29.09</v>
       </c>
-      <c r="R38" t="n">
+      <c r="T38" t="n">
         <v>-32.29000000000001</v>
       </c>
     </row>
@@ -2663,9 +2895,15 @@
         <v>-0.25</v>
       </c>
       <c r="Q39" t="n">
+        <v>5752.73848350003</v>
+      </c>
+      <c r="R39" t="n">
+        <v>-772.458183067851</v>
+      </c>
+      <c r="S39" t="n">
         <v>-19.35</v>
       </c>
-      <c r="R39" t="n">
+      <c r="T39" t="n">
         <v>-20.95</v>
       </c>
     </row>
@@ -2721,9 +2959,15 @@
         <v>-0.42</v>
       </c>
       <c r="Q40" t="n">
+        <v>6059.7627465</v>
+      </c>
+      <c r="R40" t="n">
+        <v>-1437.0404044011</v>
+      </c>
+      <c r="S40" t="n">
         <v>-34.12</v>
       </c>
-      <c r="R40" t="n">
+      <c r="T40" t="n">
         <v>-39.42</v>
       </c>
     </row>
@@ -2763,9 +3007,15 @@
         <v>-0.17</v>
       </c>
       <c r="Q41" t="n">
+        <v>6371.15275350001</v>
+      </c>
+      <c r="R41" t="n">
+        <v>-2093.21589373456</v>
+      </c>
+      <c r="S41" t="n">
         <v>-19.07</v>
       </c>
-      <c r="R41" t="n">
+      <c r="T41" t="n">
         <v>-20.47</v>
       </c>
     </row>
@@ -2817,9 +3067,15 @@
         <v>-0.17</v>
       </c>
       <c r="Q42" t="n">
+        <v>6371.15275350001</v>
+      </c>
+      <c r="R42" t="n">
+        <v>-2093.21589373456</v>
+      </c>
+      <c r="S42" t="n">
         <v>-31.77</v>
       </c>
-      <c r="R42" t="n">
+      <c r="T42" t="n">
         <v>-35.27</v>
       </c>
     </row>
@@ -2871,9 +3127,15 @@
         <v>-0.01</v>
       </c>
       <c r="Q43" t="n">
+        <v>6793.89156150003</v>
+      </c>
+      <c r="R43" t="n">
+        <v>-3388.92876440131</v>
+      </c>
+      <c r="S43" t="n">
         <v>-25.81</v>
       </c>
-      <c r="R43" t="n">
+      <c r="T43" t="n">
         <v>-27.01</v>
       </c>
     </row>
@@ -2925,9 +3187,15 @@
         <v>-0.01</v>
       </c>
       <c r="Q44" t="n">
+        <v>6793.89156150003</v>
+      </c>
+      <c r="R44" t="n">
+        <v>-3388.92876440131</v>
+      </c>
+      <c r="S44" t="n">
         <v>-27.01</v>
       </c>
-      <c r="R44" t="n">
+      <c r="T44" t="n">
         <v>-28.41</v>
       </c>
     </row>
@@ -2979,9 +3247,15 @@
         <v>0.27</v>
       </c>
       <c r="Q45" t="n">
+        <v>7237.87969050001</v>
+      </c>
+      <c r="R45" t="n">
+        <v>-4054.06297840116</v>
+      </c>
+      <c r="S45" t="n">
         <v>-23.83</v>
       </c>
-      <c r="R45" t="n">
+      <c r="T45" t="n">
         <v>-24.73</v>
       </c>
     </row>
@@ -3033,9 +3307,15 @@
         <v>0.27</v>
       </c>
       <c r="Q46" t="n">
+        <v>7237.87969050001</v>
+      </c>
+      <c r="R46" t="n">
+        <v>-4054.06297840116</v>
+      </c>
+      <c r="S46" t="n">
         <v>-24.73</v>
       </c>
-      <c r="R46" t="n">
+      <c r="T46" t="n">
         <v>-26.73</v>
       </c>
     </row>
@@ -3087,9 +3367,15 @@
         <v>0.27</v>
       </c>
       <c r="Q47" t="n">
+        <v>7237.87969050001</v>
+      </c>
+      <c r="R47" t="n">
+        <v>-4054.06297840116</v>
+      </c>
+      <c r="S47" t="n">
         <v>-26.73</v>
       </c>
-      <c r="R47" t="n">
+      <c r="T47" t="n">
         <v>-28.73</v>
       </c>
     </row>
@@ -3141,9 +3427,15 @@
         <v>0.27</v>
       </c>
       <c r="Q48" t="n">
+        <v>7237.87969050001</v>
+      </c>
+      <c r="R48" t="n">
+        <v>-4054.06297840116</v>
+      </c>
+      <c r="S48" t="n">
         <v>-28.73</v>
       </c>
-      <c r="R48" t="n">
+      <c r="T48" t="n">
         <v>-35.73</v>
       </c>
     </row>
@@ -3195,9 +3487,15 @@
         <v>-0.63</v>
       </c>
       <c r="Q49" t="n">
+        <v>7292.29018050001</v>
+      </c>
+      <c r="R49" t="n">
+        <v>-637.206354401074</v>
+      </c>
+      <c r="S49" t="n">
         <v>-29.43</v>
       </c>
-      <c r="R49" t="n">
+      <c r="T49" t="n">
         <v>-30.43</v>
       </c>
     </row>
@@ -3249,9 +3547,15 @@
         <v>-0.63</v>
       </c>
       <c r="Q50" t="n">
+        <v>7292.29018050001</v>
+      </c>
+      <c r="R50" t="n">
+        <v>-637.206354401074</v>
+      </c>
+      <c r="S50" t="n">
         <v>-32.23</v>
       </c>
-      <c r="R50" t="n">
+      <c r="T50" t="n">
         <v>-34.63</v>
       </c>
     </row>
@@ -3303,9 +3607,15 @@
         <v>-0.63</v>
       </c>
       <c r="Q51" t="n">
+        <v>7292.29018050001</v>
+      </c>
+      <c r="R51" t="n">
+        <v>-637.206354401074</v>
+      </c>
+      <c r="S51" t="n">
         <v>-34.63</v>
       </c>
-      <c r="R51" t="n">
+      <c r="T51" t="n">
         <v>-35.63</v>
       </c>
     </row>
@@ -3357,9 +3667,15 @@
         <v>-0.63</v>
       </c>
       <c r="Q52" t="n">
+        <v>7292.29018050001</v>
+      </c>
+      <c r="R52" t="n">
+        <v>-637.206354401074</v>
+      </c>
+      <c r="S52" t="n">
         <v>-35.63</v>
       </c>
-      <c r="R52" t="n">
+      <c r="T52" t="n">
         <v>-39.23</v>
       </c>
     </row>
@@ -3411,9 +3727,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q53" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R53" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S53" t="n">
         <v>-19.66</v>
       </c>
-      <c r="R53" t="n">
+      <c r="T53" t="n">
         <v>-21.56</v>
       </c>
     </row>
@@ -3465,9 +3787,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q54" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R54" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S54" t="n">
         <v>-22.76</v>
       </c>
-      <c r="R54" t="n">
+      <c r="T54" t="n">
         <v>-26.56</v>
       </c>
     </row>
@@ -3519,9 +3847,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q55" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R55" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S55" t="n">
         <v>-26.56</v>
       </c>
-      <c r="R55" t="n">
+      <c r="T55" t="n">
         <v>-27.56</v>
       </c>
     </row>
@@ -3573,9 +3907,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q56" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R56" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S56" t="n">
         <v>-27.56</v>
       </c>
-      <c r="R56" t="n">
+      <c r="T56" t="n">
         <v>-30.86</v>
       </c>
     </row>
@@ -3627,9 +3967,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q57" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R57" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S57" t="n">
         <v>-30.86</v>
       </c>
-      <c r="R57" t="n">
+      <c r="T57" t="n">
         <v>-33.36</v>
       </c>
     </row>
@@ -3681,9 +4027,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q58" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R58" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S58" t="n">
         <v>-38.46</v>
       </c>
-      <c r="R58" t="n">
+      <c r="T58" t="n">
         <v>-39.76000000000001</v>
       </c>
     </row>
@@ -3735,9 +4087,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q59" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R59" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S59" t="n">
         <v>-39.76000000000001</v>
       </c>
-      <c r="R59" t="n">
+      <c r="T59" t="n">
         <v>-42.16</v>
       </c>
     </row>
@@ -3789,9 +4147,15 @@
         <v>-0.5600000000000001</v>
       </c>
       <c r="Q60" t="n">
+        <v>7451.45790600005</v>
+      </c>
+      <c r="R60" t="n">
+        <v>-1306.94602773463</v>
+      </c>
+      <c r="S60" t="n">
         <v>-42.16</v>
       </c>
-      <c r="R60" t="n">
+      <c r="T60" t="n">
         <v>-42.96</v>
       </c>
     </row>
@@ -3843,9 +4207,15 @@
         <v>-0.59</v>
       </c>
       <c r="Q61" t="n">
+        <v>7752.92366250002</v>
+      </c>
+      <c r="R61" t="n">
+        <v>-1988.9416077345</v>
+      </c>
+      <c r="S61" t="n">
         <v>-19.89</v>
       </c>
-      <c r="R61" t="n">
+      <c r="T61" t="n">
         <v>-22.89</v>
       </c>
     </row>
@@ -3897,9 +4267,15 @@
         <v>-0.59</v>
       </c>
       <c r="Q62" t="n">
+        <v>7752.92366250002</v>
+      </c>
+      <c r="R62" t="n">
+        <v>-1988.9416077345</v>
+      </c>
+      <c r="S62" t="n">
         <v>-24.89</v>
       </c>
-      <c r="R62" t="n">
+      <c r="T62" t="n">
         <v>-26.59</v>
       </c>
     </row>
@@ -3951,9 +4327,15 @@
         <v>-0.59</v>
       </c>
       <c r="Q63" t="n">
+        <v>7752.92366250002</v>
+      </c>
+      <c r="R63" t="n">
+        <v>-1988.9416077345</v>
+      </c>
+      <c r="S63" t="n">
         <v>-26.59</v>
       </c>
-      <c r="R63" t="n">
+      <c r="T63" t="n">
         <v>-37.59</v>
       </c>
     </row>
@@ -4005,9 +4387,15 @@
         <v>-0.59</v>
       </c>
       <c r="Q64" t="n">
+        <v>7752.92366250002</v>
+      </c>
+      <c r="R64" t="n">
+        <v>-1988.9416077345</v>
+      </c>
+      <c r="S64" t="n">
         <v>-37.59</v>
       </c>
-      <c r="R64" t="n">
+      <c r="T64" t="n">
         <v>-38.59</v>
       </c>
     </row>
@@ -4059,9 +4447,15 @@
         <v>-0.43</v>
       </c>
       <c r="Q65" t="n">
+        <v>8066.72846850005</v>
+      </c>
+      <c r="R65" t="n">
+        <v>-2622.1400417344</v>
+      </c>
+      <c r="S65" t="n">
         <v>-17.93</v>
       </c>
-      <c r="R65" t="n">
+      <c r="T65" t="n">
         <v>-18.73</v>
       </c>
     </row>
@@ -4113,9 +4507,15 @@
         <v>-0.43</v>
       </c>
       <c r="Q66" t="n">
+        <v>8066.72846850005</v>
+      </c>
+      <c r="R66" t="n">
+        <v>-2622.1400417344</v>
+      </c>
+      <c r="S66" t="n">
         <v>-20.63</v>
       </c>
-      <c r="R66" t="n">
+      <c r="T66" t="n">
         <v>-21.93</v>
       </c>
     </row>
@@ -4167,9 +4567,15 @@
         <v>-0.43</v>
       </c>
       <c r="Q67" t="n">
+        <v>8066.72846850005</v>
+      </c>
+      <c r="R67" t="n">
+        <v>-2622.1400417344</v>
+      </c>
+      <c r="S67" t="n">
         <v>-26.83</v>
       </c>
-      <c r="R67" t="n">
+      <c r="T67" t="n">
         <v>-31.13</v>
       </c>
     </row>
@@ -4221,9 +4627,15 @@
         <v>-0.43</v>
       </c>
       <c r="Q68" t="n">
+        <v>8066.72846850005</v>
+      </c>
+      <c r="R68" t="n">
+        <v>-2622.1400417344</v>
+      </c>
+      <c r="S68" t="n">
         <v>-31.13</v>
       </c>
-      <c r="R68" t="n">
+      <c r="T68" t="n">
         <v>-32.63</v>
       </c>
     </row>
@@ -4275,9 +4687,15 @@
         <v>-0.42</v>
       </c>
       <c r="Q69" t="n">
+        <v>8362.94240400003</v>
+      </c>
+      <c r="R69" t="n">
+        <v>-3263.72446906784</v>
+      </c>
+      <c r="S69" t="n">
         <v>-25.62</v>
       </c>
-      <c r="R69" t="n">
+      <c r="T69" t="n">
         <v>-26.92</v>
       </c>
     </row>
@@ -4329,9 +4747,15 @@
         <v>-0.42</v>
       </c>
       <c r="Q70" t="n">
+        <v>8362.94240400003</v>
+      </c>
+      <c r="R70" t="n">
+        <v>-3263.72446906784</v>
+      </c>
+      <c r="S70" t="n">
         <v>-27.92</v>
       </c>
-      <c r="R70" t="n">
+      <c r="T70" t="n">
         <v>-29.92</v>
       </c>
     </row>
@@ -4383,9 +4807,15 @@
         <v>-0.42</v>
       </c>
       <c r="Q71" t="n">
+        <v>8362.94240400003</v>
+      </c>
+      <c r="R71" t="n">
+        <v>-3263.72446906784</v>
+      </c>
+      <c r="S71" t="n">
         <v>-30.92</v>
       </c>
-      <c r="R71" t="n">
+      <c r="T71" t="n">
         <v>-34.52</v>
       </c>
     </row>
@@ -4437,9 +4867,15 @@
         <v>-0.42</v>
       </c>
       <c r="Q72" t="n">
+        <v>8362.94240400003</v>
+      </c>
+      <c r="R72" t="n">
+        <v>-3263.72446906784</v>
+      </c>
+      <c r="S72" t="n">
         <v>-34.52</v>
       </c>
-      <c r="R72" t="n">
+      <c r="T72" t="n">
         <v>-34.92</v>
       </c>
     </row>
@@ -4491,9 +4927,15 @@
         <v>-0.04</v>
       </c>
       <c r="Q73" t="n">
+        <v>8666.779731000021</v>
+      </c>
+      <c r="R73" t="n">
+        <v>-3851.17582106777</v>
+      </c>
+      <c r="S73" t="n">
         <v>-25.14</v>
       </c>
-      <c r="R73" t="n">
+      <c r="T73" t="n">
         <v>-25.94</v>
       </c>
     </row>
@@ -4545,9 +4987,15 @@
         <v>-0.04</v>
       </c>
       <c r="Q74" t="n">
+        <v>8666.779731000021</v>
+      </c>
+      <c r="R74" t="n">
+        <v>-3851.17582106777</v>
+      </c>
+      <c r="S74" t="n">
         <v>-29.04</v>
       </c>
-      <c r="R74" t="n">
+      <c r="T74" t="n">
         <v>-33.84</v>
       </c>
     </row>
@@ -4599,9 +5047,15 @@
         <v>-3.45</v>
       </c>
       <c r="Q75" t="n">
+        <v>1414.48530750006</v>
+      </c>
+      <c r="R75" t="n">
+        <v>-4524.87822906797</v>
+      </c>
+      <c r="S75" t="n">
         <v>-24.65</v>
       </c>
-      <c r="R75" t="n">
+      <c r="T75" t="n">
         <v>-25.15</v>
       </c>
     </row>
@@ -4653,9 +5107,15 @@
         <v>-2.03</v>
       </c>
       <c r="Q76" t="n">
+        <v>1496.08111500004</v>
+      </c>
+      <c r="R76" t="n">
+        <v>-5757.87336173467</v>
+      </c>
+      <c r="S76" t="n">
         <v>-17.73</v>
       </c>
-      <c r="R76" t="n">
+      <c r="T76" t="n">
         <v>-24.03</v>
       </c>
     </row>
@@ -4707,9 +5167,15 @@
         <v>-2.03</v>
       </c>
       <c r="Q77" t="n">
+        <v>1496.08111500004</v>
+      </c>
+      <c r="R77" t="n">
+        <v>-5757.87336173467</v>
+      </c>
+      <c r="S77" t="n">
         <v>-25.03</v>
       </c>
-      <c r="R77" t="n">
+      <c r="T77" t="n">
         <v>-30.43</v>
       </c>
     </row>
@@ -4761,9 +5227,15 @@
         <v>-4.95</v>
       </c>
       <c r="Q78" t="n">
+        <v>9245.86830300005</v>
+      </c>
+      <c r="R78" t="n">
+        <v>2861.05281626557</v>
+      </c>
+      <c r="S78" t="n">
         <v>-47.25</v>
       </c>
-      <c r="R78" t="n">
+      <c r="T78" t="n">
         <v>-49.45</v>
       </c>
     </row>
@@ -4815,9 +5287,15 @@
         <v>-2.49</v>
       </c>
       <c r="Q79" t="n">
+        <v>9320.152337999991</v>
+      </c>
+      <c r="R79" t="n">
+        <v>1548.09100959885</v>
+      </c>
+      <c r="S79" t="n">
         <v>-45.49</v>
       </c>
-      <c r="R79" t="n">
+      <c r="T79" t="n">
         <v>-46.99</v>
       </c>
     </row>
@@ -4869,9 +5347,15 @@
         <v>-2.49</v>
       </c>
       <c r="Q80" t="n">
+        <v>9320.152337999991</v>
+      </c>
+      <c r="R80" t="n">
+        <v>1548.09100959885</v>
+      </c>
+      <c r="S80" t="n">
         <v>-46.99</v>
       </c>
-      <c r="R80" t="n">
+      <c r="T80" t="n">
         <v>-47.79</v>
       </c>
     </row>
@@ -4923,9 +5407,15 @@
         <v>-3.6</v>
       </c>
       <c r="Q81" t="n">
+        <v>10244.2819455</v>
+      </c>
+      <c r="R81" t="n">
+        <v>2977.90323226557</v>
+      </c>
+      <c r="S81" t="n">
         <v>-31.6</v>
       </c>
-      <c r="R81" t="n">
+      <c r="T81" t="n">
         <v>-32.6</v>
       </c>
     </row>
@@ -4977,9 +5467,15 @@
         <v>-2.52</v>
       </c>
       <c r="Q82" t="n">
+        <v>10381.4479755</v>
+      </c>
+      <c r="R82" t="n">
+        <v>2178.17618959863</v>
+      </c>
+      <c r="S82" t="n">
         <v>-42.72000000000001</v>
       </c>
-      <c r="R82" t="n">
+      <c r="T82" t="n">
         <v>-44.22000000000001</v>
       </c>
     </row>
@@ -5019,9 +5515,15 @@
         <v>-4.29</v>
       </c>
       <c r="Q83" t="n">
+        <v>10707.4287885</v>
+      </c>
+      <c r="R83" t="n">
+        <v>1656.94619759886</v>
+      </c>
+      <c r="S83" t="n">
         <v>-28.79</v>
       </c>
-      <c r="R83" t="n">
+      <c r="T83" t="n">
         <v>-30.79</v>
       </c>
     </row>
@@ -5073,9 +5575,15 @@
         <v>-4.29</v>
       </c>
       <c r="Q84" t="n">
+        <v>10707.4287885</v>
+      </c>
+      <c r="R84" t="n">
+        <v>1656.94619759886</v>
+      </c>
+      <c r="S84" t="n">
         <v>-41.19</v>
       </c>
-      <c r="R84" t="n">
+      <c r="T84" t="n">
         <v>-41.99</v>
       </c>
     </row>
@@ -5127,9 +5635,15 @@
         <v>-4.29</v>
       </c>
       <c r="Q85" t="n">
+        <v>10707.4287885</v>
+      </c>
+      <c r="R85" t="n">
+        <v>1656.94619759886</v>
+      </c>
+      <c r="S85" t="n">
         <v>-41.99</v>
       </c>
-      <c r="R85" t="n">
+      <c r="T85" t="n">
         <v>-42.79</v>
       </c>
     </row>
@@ -5181,9 +5695,15 @@
         <v>-4.29</v>
       </c>
       <c r="Q86" t="n">
+        <v>10707.4287885</v>
+      </c>
+      <c r="R86" t="n">
+        <v>1656.94619759886</v>
+      </c>
+      <c r="S86" t="n">
         <v>-44.09</v>
       </c>
-      <c r="R86" t="n">
+      <c r="T86" t="n">
         <v>-48.39</v>
       </c>
     </row>
@@ -5235,9 +5755,15 @@
         <v>-2.06</v>
       </c>
       <c r="Q87" t="n">
+        <v>11019.640611</v>
+      </c>
+      <c r="R87" t="n">
+        <v>1035.0430702654</v>
+      </c>
+      <c r="S87" t="n">
         <v>-23.06</v>
       </c>
-      <c r="R87" t="n">
+      <c r="T87" t="n">
         <v>-27.46</v>
       </c>
     </row>
@@ -5289,9 +5815,15 @@
         <v>-2.06</v>
       </c>
       <c r="Q88" t="n">
+        <v>11019.640611</v>
+      </c>
+      <c r="R88" t="n">
+        <v>1035.0430702654</v>
+      </c>
+      <c r="S88" t="n">
         <v>-27.46</v>
       </c>
-      <c r="R88" t="n">
+      <c r="T88" t="n">
         <v>-34.26000000000001</v>
       </c>
     </row>
@@ -5343,9 +5875,15 @@
         <v>-2.06</v>
       </c>
       <c r="Q89" t="n">
+        <v>11019.640611</v>
+      </c>
+      <c r="R89" t="n">
+        <v>1035.0430702654</v>
+      </c>
+      <c r="S89" t="n">
         <v>-37.46</v>
       </c>
-      <c r="R89" t="n">
+      <c r="T89" t="n">
         <v>-44.86</v>
       </c>
     </row>
@@ -5397,9 +5935,15 @@
         <v>-2.06</v>
       </c>
       <c r="Q90" t="n">
+        <v>11019.640611</v>
+      </c>
+      <c r="R90" t="n">
+        <v>1035.0430702654</v>
+      </c>
+      <c r="S90" t="n">
         <v>-44.86</v>
       </c>
-      <c r="R90" t="n">
+      <c r="T90" t="n">
         <v>-47.26000000000001</v>
       </c>
     </row>
@@ -5451,9 +5995,15 @@
         <v>-0.62</v>
       </c>
       <c r="Q91" t="n">
+        <v>11620.736073</v>
+      </c>
+      <c r="R91" t="n">
+        <v>-342.23421706787</v>
+      </c>
+      <c r="S91" t="n">
         <v>-31.12</v>
       </c>
-      <c r="R91" t="n">
+      <c r="T91" t="n">
         <v>-46.62</v>
       </c>
     </row>
@@ -5513,9 +6063,15 @@
         <v>2.27</v>
       </c>
       <c r="Q92" t="n">
+        <v>183.829200000007</v>
+      </c>
+      <c r="R92" t="n">
+        <v>458.441452265407</v>
+      </c>
+      <c r="S92" t="n">
         <v>-17.43</v>
       </c>
-      <c r="R92" t="n">
+      <c r="T92" t="n">
         <v>-18.73</v>
       </c>
     </row>
@@ -5571,9 +6127,15 @@
         <v>2.27</v>
       </c>
       <c r="Q93" t="n">
+        <v>183.829200000007</v>
+      </c>
+      <c r="R93" t="n">
+        <v>458.441452265407</v>
+      </c>
+      <c r="S93" t="n">
         <v>-22.33</v>
       </c>
-      <c r="R93" t="n">
+      <c r="T93" t="n">
         <v>-24.23</v>
       </c>
     </row>
@@ -5629,9 +6191,15 @@
         <v>2.27</v>
       </c>
       <c r="Q94" t="n">
+        <v>183.829200000007</v>
+      </c>
+      <c r="R94" t="n">
+        <v>458.441452265407</v>
+      </c>
+      <c r="S94" t="n">
         <v>-24.23</v>
       </c>
-      <c r="R94" t="n">
+      <c r="T94" t="n">
         <v>-25.03</v>
       </c>
     </row>
@@ -5687,9 +6255,15 @@
         <v>4.336</v>
       </c>
       <c r="Q95" t="n">
+        <v>7326.61470000003</v>
+      </c>
+      <c r="R95" t="n">
+        <v>-65.54454773447171</v>
+      </c>
+      <c r="S95" t="n">
         <v>-18.164</v>
       </c>
-      <c r="R95" t="n">
+      <c r="T95" t="n">
         <v>-19.864</v>
       </c>
     </row>
@@ -5745,9 +6319,15 @@
         <v>4.336</v>
       </c>
       <c r="Q96" t="n">
+        <v>7326.61470000003</v>
+      </c>
+      <c r="R96" t="n">
+        <v>-65.54454773447171</v>
+      </c>
+      <c r="S96" t="n">
         <v>-22.014</v>
       </c>
-      <c r="R96" t="n">
+      <c r="T96" t="n">
         <v>-22.664</v>
       </c>
     </row>
@@ -5803,9 +6383,15 @@
         <v>4.336</v>
       </c>
       <c r="Q97" t="n">
+        <v>7326.61470000003</v>
+      </c>
+      <c r="R97" t="n">
+        <v>-65.54454773447171</v>
+      </c>
+      <c r="S97" t="n">
         <v>-28.664</v>
       </c>
-      <c r="R97" t="n">
+      <c r="T97" t="n">
         <v>-32.814</v>
       </c>
     </row>
@@ -5865,9 +6451,15 @@
         <v>3.634</v>
       </c>
       <c r="Q98" t="n">
+        <v>3098.7537</v>
+      </c>
+      <c r="R98" t="n">
+        <v>-380.281214401126</v>
+      </c>
+      <c r="S98" t="n">
         <v>-18.366</v>
       </c>
-      <c r="R98" t="n">
+      <c r="T98" t="n">
         <v>-20.816</v>
       </c>
     </row>
@@ -5927,9 +6519,15 @@
         <v>3.778</v>
       </c>
       <c r="Q99" t="n">
+        <v>2128.21620000005</v>
+      </c>
+      <c r="R99" t="n">
+        <v>385.064118932001</v>
+      </c>
+      <c r="S99" t="n">
         <v>-23.422</v>
       </c>
-      <c r="R99" t="n">
+      <c r="T99" t="n">
         <v>-24.222</v>
       </c>
     </row>
@@ -5985,9 +6583,15 @@
         <v>3.801</v>
       </c>
       <c r="Q100" t="n">
+        <v>6966.28920000003</v>
+      </c>
+      <c r="R100" t="n">
+        <v>638.735452265479</v>
+      </c>
+      <c r="S100" t="n">
         <v>-25.999</v>
       </c>
-      <c r="R100" t="n">
+      <c r="T100" t="n">
         <v>-26.399</v>
       </c>
     </row>
@@ -6043,9 +6647,15 @@
         <v>3.801</v>
       </c>
       <c r="Q101" t="n">
+        <v>6966.28920000003</v>
+      </c>
+      <c r="R101" t="n">
+        <v>638.735452265479</v>
+      </c>
+      <c r="S101" t="n">
         <v>-28.299</v>
       </c>
-      <c r="R101" t="n">
+      <c r="T101" t="n">
         <v>-29.449</v>
       </c>
     </row>
@@ -6097,9 +6707,15 @@
         <v>3.801</v>
       </c>
       <c r="Q102" t="n">
+        <v>6966.28920000003</v>
+      </c>
+      <c r="R102" t="n">
+        <v>638.735452265479</v>
+      </c>
+      <c r="S102" t="n">
         <v>-29.449</v>
       </c>
-      <c r="R102" t="n">
+      <c r="T102" t="n">
         <v>-31.199</v>
       </c>
     </row>
@@ -6155,9 +6771,15 @@
         <v>3.801</v>
       </c>
       <c r="Q103" t="n">
+        <v>6966.28920000003</v>
+      </c>
+      <c r="R103" t="n">
+        <v>638.735452265479</v>
+      </c>
+      <c r="S103" t="n">
         <v>-31.199</v>
       </c>
-      <c r="R103" t="n">
+      <c r="T103" t="n">
         <v>-32.699</v>
       </c>
     </row>
@@ -6213,9 +6835,15 @@
         <v>3.801</v>
       </c>
       <c r="Q104" t="n">
+        <v>6966.28920000003</v>
+      </c>
+      <c r="R104" t="n">
+        <v>638.735452265479</v>
+      </c>
+      <c r="S104" t="n">
         <v>-32.699</v>
       </c>
-      <c r="R104" t="n">
+      <c r="T104" t="n">
         <v>-34.099</v>
       </c>
     </row>
@@ -6271,9 +6899,15 @@
         <v>3.801</v>
       </c>
       <c r="Q105" t="n">
+        <v>6966.28920000003</v>
+      </c>
+      <c r="R105" t="n">
+        <v>638.735452265479</v>
+      </c>
+      <c r="S105" t="n">
         <v>-34.099</v>
       </c>
-      <c r="R105" t="n">
+      <c r="T105" t="n">
         <v>-35.899</v>
       </c>
     </row>
@@ -6333,9 +6967,15 @@
         <v>1.615</v>
       </c>
       <c r="Q106" t="n">
+        <v>-139.644299999956</v>
+      </c>
+      <c r="R106" t="n">
+        <v>2981.97611893217</v>
+      </c>
+      <c r="S106" t="n">
         <v>-19.585</v>
       </c>
-      <c r="R106" t="n">
+      <c r="T106" t="n">
         <v>-20.285</v>
       </c>
     </row>
@@ -6395,9 +7035,15 @@
         <v>2.54</v>
       </c>
       <c r="Q107" t="n">
+        <v>1860.6912</v>
+      </c>
+      <c r="R107" t="n">
+        <v>1265.46478559884</v>
+      </c>
+      <c r="S107" t="n">
         <v>-21.26</v>
       </c>
-      <c r="R107" t="n">
+      <c r="T107" t="n">
         <v>-21.66</v>
       </c>
     </row>
@@ -6453,9 +7099,15 @@
         <v>3.389</v>
       </c>
       <c r="Q108" t="n">
+        <v>1848.01770000005</v>
+      </c>
+      <c r="R108" t="n">
+        <v>2464.18278559887</v>
+      </c>
+      <c r="S108" t="n">
         <v>-28.711</v>
       </c>
-      <c r="R108" t="n">
+      <c r="T108" t="n">
         <v>-29.811</v>
       </c>
     </row>
@@ -6511,9 +7163,15 @@
         <v>3.389</v>
       </c>
       <c r="Q109" t="n">
+        <v>1848.01770000005</v>
+      </c>
+      <c r="R109" t="n">
+        <v>2464.18278559887</v>
+      </c>
+      <c r="S109" t="n">
         <v>-30.461</v>
       </c>
-      <c r="R109" t="n">
+      <c r="T109" t="n">
         <v>-30.911</v>
       </c>
     </row>
@@ -6573,9 +7231,15 @@
         <v>3.389</v>
       </c>
       <c r="Q110" t="n">
+        <v>1848.01770000005</v>
+      </c>
+      <c r="R110" t="n">
+        <v>2464.18278559887</v>
+      </c>
+      <c r="S110" t="n">
         <v>-31.711</v>
       </c>
-      <c r="R110" t="n">
+      <c r="T110" t="n">
         <v>-32.48099999999999</v>
       </c>
     </row>
@@ -6631,9 +7295,15 @@
         <v>3.288</v>
       </c>
       <c r="Q111" t="n">
+        <v>2734.27770000001</v>
+      </c>
+      <c r="R111" t="n">
+        <v>2505.25545226534</v>
+      </c>
+      <c r="S111" t="n">
         <v>-38.562</v>
       </c>
-      <c r="R111" t="n">
+      <c r="T111" t="n">
         <v>-38.862</v>
       </c>
     </row>
@@ -6693,9 +7363,15 @@
         <v>1.738</v>
       </c>
       <c r="Q112" t="n">
+        <v>4666.26120000001</v>
+      </c>
+      <c r="R112" t="n">
+        <v>2633.77878559877</v>
+      </c>
+      <c r="S112" t="n">
         <v>-18.962</v>
       </c>
-      <c r="R112" t="n">
+      <c r="T112" t="n">
         <v>-24.262</v>
       </c>
     </row>
@@ -6751,9 +7427,15 @@
         <v>1.738</v>
       </c>
       <c r="Q113" t="n">
+        <v>4666.26120000001</v>
+      </c>
+      <c r="R113" t="n">
+        <v>2633.77878559877</v>
+      </c>
+      <c r="S113" t="n">
         <v>-29.462</v>
       </c>
-      <c r="R113" t="n">
+      <c r="T113" t="n">
         <v>-29.962</v>
       </c>
     </row>
@@ -6809,9 +7491,15 @@
         <v>1.738</v>
       </c>
       <c r="Q114" t="n">
+        <v>4666.26120000001</v>
+      </c>
+      <c r="R114" t="n">
+        <v>2633.77878559877</v>
+      </c>
+      <c r="S114" t="n">
         <v>-30.262</v>
       </c>
-      <c r="R114" t="n">
+      <c r="T114" t="n">
         <v>-31.062</v>
       </c>
     </row>
@@ -6871,9 +7559,15 @@
         <v>1.738</v>
       </c>
       <c r="Q115" t="n">
+        <v>4666.26120000001</v>
+      </c>
+      <c r="R115" t="n">
+        <v>2633.77878559877</v>
+      </c>
+      <c r="S115" t="n">
         <v>-31.062</v>
       </c>
-      <c r="R115" t="n">
+      <c r="T115" t="n">
         <v>-35.062</v>
       </c>
     </row>
@@ -6929,9 +7623,15 @@
         <v>1.738</v>
       </c>
       <c r="Q116" t="n">
+        <v>4666.26120000001</v>
+      </c>
+      <c r="R116" t="n">
+        <v>2633.77878559877</v>
+      </c>
+      <c r="S116" t="n">
         <v>-35.062</v>
       </c>
-      <c r="R116" t="n">
+      <c r="T116" t="n">
         <v>-36.062</v>
       </c>
     </row>
@@ -6987,9 +7687,15 @@
         <v>1.738</v>
       </c>
       <c r="Q117" t="n">
+        <v>4666.26120000001</v>
+      </c>
+      <c r="R117" t="n">
+        <v>2633.77878559877</v>
+      </c>
+      <c r="S117" t="n">
         <v>-36.062</v>
       </c>
-      <c r="R117" t="n">
+      <c r="T117" t="n">
         <v>-37.862</v>
       </c>
     </row>
@@ -7045,9 +7751,15 @@
         <v>1.738</v>
       </c>
       <c r="Q118" t="n">
+        <v>4666.26120000001</v>
+      </c>
+      <c r="R118" t="n">
+        <v>2633.77878559877</v>
+      </c>
+      <c r="S118" t="n">
         <v>-37.862</v>
       </c>
-      <c r="R118" t="n">
+      <c r="T118" t="n">
         <v>-38.762</v>
       </c>
     </row>
@@ -7103,9 +7815,15 @@
         <v>4.426</v>
       </c>
       <c r="Q119" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R119" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S119" t="n">
         <v>-19.674</v>
       </c>
-      <c r="R119" t="n">
+      <c r="T119" t="n">
         <v>-20.574</v>
       </c>
     </row>
@@ -7161,9 +7879,15 @@
         <v>4.426</v>
       </c>
       <c r="Q120" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R120" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S120" t="n">
         <v>-20.574</v>
       </c>
-      <c r="R120" t="n">
+      <c r="T120" t="n">
         <v>-23.374</v>
       </c>
     </row>
@@ -7219,9 +7943,15 @@
         <v>4.426</v>
       </c>
       <c r="Q121" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R121" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S121" t="n">
         <v>-23.374</v>
       </c>
-      <c r="R121" t="n">
+      <c r="T121" t="n">
         <v>-25.324</v>
       </c>
     </row>
@@ -7281,9 +8011,15 @@
         <v>4.426</v>
       </c>
       <c r="Q122" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R122" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S122" t="n">
         <v>-25.324</v>
       </c>
-      <c r="R122" t="n">
+      <c r="T122" t="n">
         <v>-27.674</v>
       </c>
     </row>
@@ -7343,9 +8079,15 @@
         <v>4.426</v>
       </c>
       <c r="Q123" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R123" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S123" t="n">
         <v>-27.674</v>
       </c>
-      <c r="R123" t="n">
+      <c r="T123" t="n">
         <v>-29.724</v>
       </c>
     </row>
@@ -7401,9 +8143,15 @@
         <v>4.426</v>
       </c>
       <c r="Q124" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R124" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S124" t="n">
         <v>-29.724</v>
       </c>
-      <c r="R124" t="n">
+      <c r="T124" t="n">
         <v>-30.574</v>
       </c>
     </row>
@@ -7463,9 +8211,15 @@
         <v>4.426</v>
       </c>
       <c r="Q125" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R125" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S125" t="n">
         <v>-30.574</v>
       </c>
-      <c r="R125" t="n">
+      <c r="T125" t="n">
         <v>-32.174</v>
       </c>
     </row>
@@ -7521,9 +8275,15 @@
         <v>4.426</v>
       </c>
       <c r="Q126" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R126" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S126" t="n">
         <v>-32.174</v>
       </c>
-      <c r="R126" t="n">
+      <c r="T126" t="n">
         <v>-36.244</v>
       </c>
     </row>
@@ -7579,9 +8339,15 @@
         <v>4.426</v>
       </c>
       <c r="Q127" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R127" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S127" t="n">
         <v>-36.244</v>
       </c>
-      <c r="R127" t="n">
+      <c r="T127" t="n">
         <v>-40.274</v>
       </c>
     </row>
@@ -7637,9 +8403,15 @@
         <v>4.426</v>
       </c>
       <c r="Q128" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R128" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S128" t="n">
         <v>-40.274</v>
       </c>
-      <c r="R128" t="n">
+      <c r="T128" t="n">
         <v>-41.574</v>
       </c>
     </row>
@@ -7695,9 +8467,15 @@
         <v>4.426</v>
       </c>
       <c r="Q129" t="n">
+        <v>6821.54820000002</v>
+      </c>
+      <c r="R129" t="n">
+        <v>2691.48811893196</v>
+      </c>
+      <c r="S129" t="n">
         <v>-41.574</v>
       </c>
-      <c r="R129" t="n">
+      <c r="T129" t="n">
         <v>-44.574</v>
       </c>
     </row>
@@ -7753,9 +8531,15 @@
         <v>1.898</v>
       </c>
       <c r="Q130" t="n">
+        <v>217.160700000037</v>
+      </c>
+      <c r="R130" t="n">
+        <v>1754.27678559876</v>
+      </c>
+      <c r="S130" t="n">
         <v>-15.202</v>
       </c>
-      <c r="R130" t="n">
+      <c r="T130" t="n">
         <v>-17.302</v>
       </c>
     </row>
@@ -7811,9 +8595,15 @@
         <v>1.898</v>
       </c>
       <c r="Q131" t="n">
+        <v>217.160700000037</v>
+      </c>
+      <c r="R131" t="n">
+        <v>1754.27678559876</v>
+      </c>
+      <c r="S131" t="n">
         <v>-30.902</v>
       </c>
-      <c r="R131" t="n">
+      <c r="T131" t="n">
         <v>-33.102</v>
       </c>
     </row>
@@ -7869,9 +8659,15 @@
         <v>2.865</v>
       </c>
       <c r="Q132" t="n">
+        <v>2023.84770000001</v>
+      </c>
+      <c r="R132" t="n">
+        <v>4165.22278559891</v>
+      </c>
+      <c r="S132" t="n">
         <v>-16.935</v>
       </c>
-      <c r="R132" t="n">
+      <c r="T132" t="n">
         <v>-18.035</v>
       </c>
     </row>
@@ -7927,9 +8723,15 @@
         <v>3.26</v>
       </c>
       <c r="Q133" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R133" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S133" t="n">
         <v>-24.24</v>
       </c>
-      <c r="R133" t="n">
+      <c r="T133" t="n">
         <v>-25.14</v>
       </c>
     </row>
@@ -7985,9 +8787,15 @@
         <v>3.26</v>
       </c>
       <c r="Q134" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R134" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S134" t="n">
         <v>-25.14</v>
       </c>
-      <c r="R134" t="n">
+      <c r="T134" t="n">
         <v>-26.74</v>
       </c>
     </row>
@@ -8039,9 +8847,15 @@
         <v>3.26</v>
       </c>
       <c r="Q135" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R135" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S135" t="n">
         <v>-27.24</v>
       </c>
-      <c r="R135" t="n">
+      <c r="T135" t="n">
         <v>-29.74</v>
       </c>
     </row>
@@ -8093,9 +8907,15 @@
         <v>3.26</v>
       </c>
       <c r="Q136" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R136" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S136" t="n">
         <v>-29.74</v>
       </c>
-      <c r="R136" t="n">
+      <c r="T136" t="n">
         <v>-31.49</v>
       </c>
     </row>
@@ -8151,9 +8971,15 @@
         <v>3.26</v>
       </c>
       <c r="Q137" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R137" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S137" t="n">
         <v>-31.49</v>
       </c>
-      <c r="R137" t="n">
+      <c r="T137" t="n">
         <v>-36.34</v>
       </c>
     </row>
@@ -8209,9 +9035,15 @@
         <v>3.26</v>
       </c>
       <c r="Q138" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R138" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S138" t="n">
         <v>-36.34</v>
       </c>
-      <c r="R138" t="n">
+      <c r="T138" t="n">
         <v>-37.44</v>
       </c>
     </row>
@@ -8267,9 +9099,15 @@
         <v>3.26</v>
       </c>
       <c r="Q139" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R139" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S139" t="n">
         <v>-42.29</v>
       </c>
-      <c r="R139" t="n">
+      <c r="T139" t="n">
         <v>-43.24</v>
       </c>
     </row>
@@ -8325,9 +9163,15 @@
         <v>3.26</v>
       </c>
       <c r="Q140" t="n">
+        <v>5332.17120000001</v>
+      </c>
+      <c r="R140" t="n">
+        <v>3887.00078559884</v>
+      </c>
+      <c r="S140" t="n">
         <v>-43.24</v>
       </c>
-      <c r="R140" t="n">
+      <c r="T140" t="n">
         <v>-49.94</v>
       </c>
     </row>
@@ -8387,9 +9231,15 @@
         <v>4.153</v>
       </c>
       <c r="Q141" t="n">
+        <v>6420.39720000001</v>
+      </c>
+      <c r="R141" t="n">
+        <v>3856.97678559863</v>
+      </c>
+      <c r="S141" t="n">
         <v>-19.147</v>
       </c>
-      <c r="R141" t="n">
+      <c r="T141" t="n">
         <v>-20.147</v>
       </c>
     </row>
@@ -8449,9 +9299,15 @@
         <v>4.153</v>
       </c>
       <c r="Q142" t="n">
+        <v>6420.39720000001</v>
+      </c>
+      <c r="R142" t="n">
+        <v>3856.97678559863</v>
+      </c>
+      <c r="S142" t="n">
         <v>-20.147</v>
       </c>
-      <c r="R142" t="n">
+      <c r="T142" t="n">
         <v>-23.447</v>
       </c>
     </row>
@@ -8507,9 +9363,15 @@
         <v>4.153</v>
       </c>
       <c r="Q143" t="n">
+        <v>6420.39720000001</v>
+      </c>
+      <c r="R143" t="n">
+        <v>3856.97678559863</v>
+      </c>
+      <c r="S143" t="n">
         <v>-28.147</v>
       </c>
-      <c r="R143" t="n">
+      <c r="T143" t="n">
         <v>-29.647</v>
       </c>
     </row>
@@ -8565,9 +9427,15 @@
         <v>4.153</v>
       </c>
       <c r="Q144" t="n">
+        <v>6420.39720000001</v>
+      </c>
+      <c r="R144" t="n">
+        <v>3856.97678559863</v>
+      </c>
+      <c r="S144" t="n">
         <v>-29.647</v>
       </c>
-      <c r="R144" t="n">
+      <c r="T144" t="n">
         <v>-31.047</v>
       </c>
     </row>
@@ -8623,9 +9491,15 @@
         <v>4.153</v>
       </c>
       <c r="Q145" t="n">
+        <v>6420.39720000001</v>
+      </c>
+      <c r="R145" t="n">
+        <v>3856.97678559863</v>
+      </c>
+      <c r="S145" t="n">
         <v>-34.147</v>
       </c>
-      <c r="R145" t="n">
+      <c r="T145" t="n">
         <v>-37.747</v>
       </c>
     </row>
@@ -8681,9 +9555,15 @@
         <v>4.153</v>
       </c>
       <c r="Q146" t="n">
+        <v>6420.39720000001</v>
+      </c>
+      <c r="R146" t="n">
+        <v>3856.97678559863</v>
+      </c>
+      <c r="S146" t="n">
         <v>-39.997</v>
       </c>
-      <c r="R146" t="n">
+      <c r="T146" t="n">
         <v>-40.147</v>
       </c>
     </row>
@@ -8739,9 +9619,15 @@
         <v>4.153</v>
       </c>
       <c r="Q147" t="n">
+        <v>6420.39720000001</v>
+      </c>
+      <c r="R147" t="n">
+        <v>3856.97678559863</v>
+      </c>
+      <c r="S147" t="n">
         <v>-46.847</v>
       </c>
-      <c r="R147" t="n">
+      <c r="T147" t="n">
         <v>-49.647</v>
       </c>
     </row>
@@ -8797,9 +9683,15 @@
         <v>3.536</v>
       </c>
       <c r="Q148" t="n">
+        <v>5722.62570000003</v>
+      </c>
+      <c r="R148" t="n">
+        <v>4466.66211893223</v>
+      </c>
+      <c r="S148" t="n">
         <v>-24.564</v>
       </c>
-      <c r="R148" t="n">
+      <c r="T148" t="n">
         <v>-25.064</v>
       </c>
     </row>
@@ -8855,9 +9747,15 @@
         <v>3.536</v>
       </c>
       <c r="Q149" t="n">
+        <v>5722.62570000003</v>
+      </c>
+      <c r="R149" t="n">
+        <v>4466.66211893223</v>
+      </c>
+      <c r="S149" t="n">
         <v>-25.764</v>
       </c>
-      <c r="R149" t="n">
+      <c r="T149" t="n">
         <v>-26.764</v>
       </c>
     </row>
@@ -8913,9 +9811,15 @@
         <v>3.536</v>
       </c>
       <c r="Q150" t="n">
+        <v>5722.62570000003</v>
+      </c>
+      <c r="R150" t="n">
+        <v>4466.66211893223</v>
+      </c>
+      <c r="S150" t="n">
         <v>-26.764</v>
       </c>
-      <c r="R150" t="n">
+      <c r="T150" t="n">
         <v>-29.564</v>
       </c>
     </row>
@@ -8971,9 +9875,15 @@
         <v>3.536</v>
       </c>
       <c r="Q151" t="n">
+        <v>5722.62570000003</v>
+      </c>
+      <c r="R151" t="n">
+        <v>4466.66211893223</v>
+      </c>
+      <c r="S151" t="n">
         <v>-31.864</v>
       </c>
-      <c r="R151" t="n">
+      <c r="T151" t="n">
         <v>-33.664</v>
       </c>
     </row>
@@ -9029,9 +9939,15 @@
         <v>3.536</v>
       </c>
       <c r="Q152" t="n">
+        <v>5722.62570000003</v>
+      </c>
+      <c r="R152" t="n">
+        <v>4466.66211893223</v>
+      </c>
+      <c r="S152" t="n">
         <v>-33.664</v>
       </c>
-      <c r="R152" t="n">
+      <c r="T152" t="n">
         <v>-46.564</v>
       </c>
     </row>
@@ -9087,9 +10003,15 @@
         <v>3.959</v>
       </c>
       <c r="Q153" t="n">
+        <v>4750.63920000006</v>
+      </c>
+      <c r="R153" t="n">
+        <v>4916.19211893218</v>
+      </c>
+      <c r="S153" t="n">
         <v>-27.541</v>
       </c>
-      <c r="R153" t="n">
+      <c r="T153" t="n">
         <v>-32.541</v>
       </c>
     </row>
@@ -9145,9 +10067,15 @@
         <v>3.959</v>
       </c>
       <c r="Q154" t="n">
+        <v>4750.63920000006</v>
+      </c>
+      <c r="R154" t="n">
+        <v>4916.19211893218</v>
+      </c>
+      <c r="S154" t="n">
         <v>-32.84099999999999</v>
       </c>
-      <c r="R154" t="n">
+      <c r="T154" t="n">
         <v>-35.34099999999999</v>
       </c>
     </row>
@@ -9203,9 +10131,15 @@
         <v>3.959</v>
       </c>
       <c r="Q155" t="n">
+        <v>4750.63920000006</v>
+      </c>
+      <c r="R155" t="n">
+        <v>4916.19211893218</v>
+      </c>
+      <c r="S155" t="n">
         <v>-35.641</v>
       </c>
-      <c r="R155" t="n">
+      <c r="T155" t="n">
         <v>-36.34099999999999</v>
       </c>
     </row>
@@ -9261,9 +10195,15 @@
         <v>3.959</v>
       </c>
       <c r="Q156" t="n">
+        <v>4750.63920000006</v>
+      </c>
+      <c r="R156" t="n">
+        <v>4916.19211893218</v>
+      </c>
+      <c r="S156" t="n">
         <v>-39.641</v>
       </c>
-      <c r="R156" t="n">
+      <c r="T156" t="n">
         <v>-41.441</v>
       </c>
     </row>
@@ -9319,9 +10259,15 @@
         <v>2.706</v>
       </c>
       <c r="Q157" t="n">
+        <v>4588.13370000006</v>
+      </c>
+      <c r="R157" t="n">
+        <v>4583.84345226549</v>
+      </c>
+      <c r="S157" t="n">
         <v>-21.394</v>
       </c>
-      <c r="R157" t="n">
+      <c r="T157" t="n">
         <v>-23.794</v>
       </c>
     </row>
@@ -9377,9 +10323,15 @@
         <v>2.706</v>
       </c>
       <c r="Q158" t="n">
+        <v>4588.13370000006</v>
+      </c>
+      <c r="R158" t="n">
+        <v>4583.84345226549</v>
+      </c>
+      <c r="S158" t="n">
         <v>-23.994</v>
       </c>
-      <c r="R158" t="n">
+      <c r="T158" t="n">
         <v>-24.794</v>
       </c>
     </row>
@@ -9435,9 +10387,15 @@
         <v>2.706</v>
       </c>
       <c r="Q159" t="n">
+        <v>4588.13370000006</v>
+      </c>
+      <c r="R159" t="n">
+        <v>4583.84345226549</v>
+      </c>
+      <c r="S159" t="n">
         <v>-25.294</v>
       </c>
-      <c r="R159" t="n">
+      <c r="T159" t="n">
         <v>-25.994</v>
       </c>
     </row>
@@ -9493,9 +10451,15 @@
         <v>2.706</v>
       </c>
       <c r="Q160" t="n">
+        <v>4588.13370000006</v>
+      </c>
+      <c r="R160" t="n">
+        <v>4583.84345226549</v>
+      </c>
+      <c r="S160" t="n">
         <v>-26.994</v>
       </c>
-      <c r="R160" t="n">
+      <c r="T160" t="n">
         <v>-29.694</v>
       </c>
     </row>
@@ -9555,9 +10519,15 @@
         <v>2.706</v>
       </c>
       <c r="Q161" t="n">
+        <v>4588.13370000006</v>
+      </c>
+      <c r="R161" t="n">
+        <v>4583.84345226549</v>
+      </c>
+      <c r="S161" t="n">
         <v>-29.694</v>
       </c>
-      <c r="R161" t="n">
+      <c r="T161" t="n">
         <v>-33.294</v>
       </c>
     </row>
@@ -9613,9 +10583,15 @@
         <v>2.706</v>
       </c>
       <c r="Q162" t="n">
+        <v>4588.13370000006</v>
+      </c>
+      <c r="R162" t="n">
+        <v>4583.84345226549</v>
+      </c>
+      <c r="S162" t="n">
         <v>-33.294</v>
       </c>
-      <c r="R162" t="n">
+      <c r="T162" t="n">
         <v>-34.294</v>
       </c>
     </row>
@@ -9671,9 +10647,15 @@
         <v>3.781</v>
       </c>
       <c r="Q163" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R163" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S163" t="n">
         <v>-17.119</v>
       </c>
-      <c r="R163" t="n">
+      <c r="T163" t="n">
         <v>-21.219</v>
       </c>
     </row>
@@ -9729,9 +10711,15 @@
         <v>3.781</v>
       </c>
       <c r="Q164" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R164" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S164" t="n">
         <v>-22.619</v>
       </c>
-      <c r="R164" t="n">
+      <c r="T164" t="n">
         <v>-23.019</v>
       </c>
     </row>
@@ -9791,9 +10779,15 @@
         <v>3.781</v>
       </c>
       <c r="Q165" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R165" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S165" t="n">
         <v>-26.219</v>
       </c>
-      <c r="R165" t="n">
+      <c r="T165" t="n">
         <v>-26.519</v>
       </c>
     </row>
@@ -9849,9 +10843,15 @@
         <v>3.781</v>
       </c>
       <c r="Q166" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R166" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S166" t="n">
         <v>-27.019</v>
       </c>
-      <c r="R166" t="n">
+      <c r="T166" t="n">
         <v>-29.419</v>
       </c>
     </row>
@@ -9907,9 +10907,15 @@
         <v>3.781</v>
       </c>
       <c r="Q167" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R167" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S167" t="n">
         <v>-29.419</v>
       </c>
-      <c r="R167" t="n">
+      <c r="T167" t="n">
         <v>-30.519</v>
       </c>
     </row>
@@ -9965,9 +10971,15 @@
         <v>3.781</v>
       </c>
       <c r="Q168" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R168" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S168" t="n">
         <v>-30.519</v>
       </c>
-      <c r="R168" t="n">
+      <c r="T168" t="n">
         <v>-31.119</v>
       </c>
     </row>
@@ -10023,9 +11035,15 @@
         <v>3.781</v>
       </c>
       <c r="Q169" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R169" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S169" t="n">
         <v>-33.319</v>
       </c>
-      <c r="R169" t="n">
+      <c r="T169" t="n">
         <v>-35.619</v>
       </c>
     </row>
@@ -10081,9 +11099,15 @@
         <v>3.781</v>
       </c>
       <c r="Q170" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R170" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S170" t="n">
         <v>-35.619</v>
       </c>
-      <c r="R170" t="n">
+      <c r="T170" t="n">
         <v>-38.919</v>
       </c>
     </row>
@@ -10139,9 +11163,15 @@
         <v>3.781</v>
       </c>
       <c r="Q171" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R171" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S171" t="n">
         <v>-38.919</v>
       </c>
-      <c r="R171" t="n">
+      <c r="T171" t="n">
         <v>-40.519</v>
       </c>
     </row>
@@ -10197,9 +11227,15 @@
         <v>3.781</v>
       </c>
       <c r="Q172" t="n">
+        <v>3489.26670000001</v>
+      </c>
+      <c r="R172" t="n">
+        <v>5070.16945226553</v>
+      </c>
+      <c r="S172" t="n">
         <v>-46.319</v>
       </c>
-      <c r="R172" t="n">
+      <c r="T172" t="n">
         <v>-49.219</v>
       </c>
     </row>
@@ -10259,9 +11295,15 @@
         <v>3.238</v>
       </c>
       <c r="Q173" t="n">
+        <v>3398.29920000007</v>
+      </c>
+      <c r="R173" t="n">
+        <v>5448.07678559888</v>
+      </c>
+      <c r="S173" t="n">
         <v>-15.212</v>
       </c>
-      <c r="R173" t="n">
+      <c r="T173" t="n">
         <v>-21.462</v>
       </c>
     </row>
@@ -10317,9 +11359,15 @@
         <v>3.238</v>
       </c>
       <c r="Q174" t="n">
+        <v>3398.29920000007</v>
+      </c>
+      <c r="R174" t="n">
+        <v>5448.07678559888</v>
+      </c>
+      <c r="S174" t="n">
         <v>-27.362</v>
       </c>
-      <c r="R174" t="n">
+      <c r="T174" t="n">
         <v>-28.812</v>
       </c>
     </row>
@@ -10375,9 +11423,15 @@
         <v>3.238</v>
       </c>
       <c r="Q175" t="n">
+        <v>3398.29920000007</v>
+      </c>
+      <c r="R175" t="n">
+        <v>5448.07678559888</v>
+      </c>
+      <c r="S175" t="n">
         <v>-32.512</v>
       </c>
-      <c r="R175" t="n">
+      <c r="T175" t="n">
         <v>-33.002</v>
       </c>
     </row>
@@ -10437,9 +11491,15 @@
         <v>3.238</v>
       </c>
       <c r="Q176" t="n">
+        <v>3398.29920000007</v>
+      </c>
+      <c r="R176" t="n">
+        <v>5448.07678559888</v>
+      </c>
+      <c r="S176" t="n">
         <v>-33.412</v>
       </c>
-      <c r="R176" t="n">
+      <c r="T176" t="n">
         <v>-39.612</v>
       </c>
     </row>
@@ -10495,9 +11555,15 @@
         <v>3.238</v>
       </c>
       <c r="Q177" t="n">
+        <v>3398.29920000007</v>
+      </c>
+      <c r="R177" t="n">
+        <v>5448.07678559888</v>
+      </c>
+      <c r="S177" t="n">
         <v>-39.612</v>
       </c>
-      <c r="R177" t="n">
+      <c r="T177" t="n">
         <v>-41.192</v>
       </c>
     </row>
@@ -10553,9 +11619,15 @@
         <v>3.238</v>
       </c>
       <c r="Q178" t="n">
+        <v>3398.29920000007</v>
+      </c>
+      <c r="R178" t="n">
+        <v>5448.07678559888</v>
+      </c>
+      <c r="S178" t="n">
         <v>-41.192</v>
       </c>
-      <c r="R178" t="n">
+      <c r="T178" t="n">
         <v>-42.162</v>
       </c>
     </row>
@@ -10611,9 +11683,15 @@
         <v>3.238</v>
       </c>
       <c r="Q179" t="n">
+        <v>3398.29920000007</v>
+      </c>
+      <c r="R179" t="n">
+        <v>5448.07678559888</v>
+      </c>
+      <c r="S179" t="n">
         <v>-42.162</v>
       </c>
-      <c r="R179" t="n">
+      <c r="T179" t="n">
         <v>-46.962</v>
       </c>
     </row>
@@ -10673,9 +11751,15 @@
         <v>4.36</v>
       </c>
       <c r="Q180" t="n">
+        <v>5182.68120000005</v>
+      </c>
+      <c r="R180" t="n">
+        <v>952.399452265352</v>
+      </c>
+      <c r="S180" t="n">
         <v>-15.44</v>
       </c>
-      <c r="R180" t="n">
+      <c r="T180" t="n">
         <v>-17.2</v>
       </c>
     </row>
@@ -10731,9 +11815,15 @@
         <v>3.608</v>
       </c>
       <c r="Q181" t="n">
+        <v>318.536699999997</v>
+      </c>
+      <c r="R181" t="n">
+        <v>5478.78411893205</v>
+      </c>
+      <c r="S181" t="n">
         <v>-34.192</v>
       </c>
-      <c r="R181" t="n">
+      <c r="T181" t="n">
         <v>-35.892</v>
       </c>
     </row>
@@ -10789,9 +11879,15 @@
         <v>3.738</v>
       </c>
       <c r="Q182" t="n">
+        <v>-1859.17079999999</v>
+      </c>
+      <c r="R182" t="n">
+        <v>4805.06678559879</v>
+      </c>
+      <c r="S182" t="n">
         <v>-26.962</v>
       </c>
-      <c r="R182" t="n">
+      <c r="T182" t="n">
         <v>-28.262</v>
       </c>
     </row>
@@ -10847,9 +11943,15 @@
         <v>3.411</v>
       </c>
       <c r="Q183" t="n">
+        <v>-1361.55779999995</v>
+      </c>
+      <c r="R183" t="n">
+        <v>1471.4654522653</v>
+      </c>
+      <c r="S183" t="n">
         <v>-15.989</v>
       </c>
-      <c r="R183" t="n">
+      <c r="T183" t="n">
         <v>-17.589</v>
       </c>
     </row>
@@ -10905,9 +12007,15 @@
         <v>3.411</v>
       </c>
       <c r="Q184" t="n">
+        <v>-1361.55779999995</v>
+      </c>
+      <c r="R184" t="n">
+        <v>1471.4654522653</v>
+      </c>
+      <c r="S184" t="n">
         <v>-23.689</v>
       </c>
-      <c r="R184" t="n">
+      <c r="T184" t="n">
         <v>-25.289</v>
       </c>
     </row>
@@ -10963,9 +12071,15 @@
         <v>3.908</v>
       </c>
       <c r="Q185" t="n">
+        <v>455.123700000026</v>
+      </c>
+      <c r="R185" t="n">
+        <v>-2997.43721440124</v>
+      </c>
+      <c r="S185" t="n">
         <v>-19.692</v>
       </c>
-      <c r="R185" t="n">
+      <c r="T185" t="n">
         <v>-25.392</v>
       </c>
     </row>
@@ -11021,9 +12135,15 @@
         <v>2.766</v>
       </c>
       <c r="Q186" t="n">
+        <v>164.984700000059</v>
+      </c>
+      <c r="R186" t="n">
+        <v>-4267.22388106802</v>
+      </c>
+      <c r="S186" t="n">
         <v>-19.234</v>
       </c>
-      <c r="R186" t="n">
+      <c r="T186" t="n">
         <v>-20.034</v>
       </c>
     </row>
@@ -11071,9 +12191,15 @@
         <v>4.576</v>
       </c>
       <c r="Q187" t="n">
+        <v>5692.32570000002</v>
+      </c>
+      <c r="R187" t="n">
+        <v>6535.87278559866</v>
+      </c>
+      <c r="S187" t="n">
         <v>-29.924</v>
       </c>
-      <c r="R187" t="n">
+      <c r="T187" t="n">
         <v>-42.674</v>
       </c>
     </row>
@@ -11129,9 +12255,15 @@
         <v>4.576</v>
       </c>
       <c r="Q188" t="n">
+        <v>5692.32570000002</v>
+      </c>
+      <c r="R188" t="n">
+        <v>6535.87278559866</v>
+      </c>
+      <c r="S188" t="n">
         <v>-42.674</v>
       </c>
-      <c r="R188" t="n">
+      <c r="T188" t="n">
         <v>-48.424</v>
       </c>
     </row>
@@ -11183,9 +12315,15 @@
         <v>4.576</v>
       </c>
       <c r="Q189" t="n">
+        <v>5692.32570000002</v>
+      </c>
+      <c r="R189" t="n">
+        <v>6535.87278559866</v>
+      </c>
+      <c r="S189" t="n">
         <v>-48.424</v>
       </c>
-      <c r="R189" t="n">
+      <c r="T189" t="n">
         <v>-49.424</v>
       </c>
     </row>
@@ -11245,9 +12383,15 @@
         <v>6.797</v>
       </c>
       <c r="Q190" t="n">
+        <v>1593.23220000003</v>
+      </c>
+      <c r="R190" t="n">
+        <v>5589.67611893204</v>
+      </c>
+      <c r="S190" t="n">
         <v>-18.203</v>
       </c>
-      <c r="R190" t="n">
+      <c r="T190" t="n">
         <v>-22.103</v>
       </c>
     </row>
@@ -11303,9 +12447,15 @@
         <v>3.458</v>
       </c>
       <c r="Q191" t="n">
+        <v>-2449.40879999995</v>
+      </c>
+      <c r="R191" t="n">
+        <v>5338.31478559878</v>
+      </c>
+      <c r="S191" t="n">
         <v>-36.342</v>
       </c>
-      <c r="R191" t="n">
+      <c r="T191" t="n">
         <v>-39.542</v>
       </c>
     </row>
@@ -11361,9 +12511,15 @@
         <v>4</v>
       </c>
       <c r="Q192" t="n">
+        <v>2931.17970000007</v>
+      </c>
+      <c r="R192" t="n">
+        <v>4928.08011893214</v>
+      </c>
+      <c r="S192" t="n">
         <v>-34</v>
       </c>
-      <c r="R192" t="n">
+      <c r="T192" t="n">
         <v>-36</v>
       </c>
     </row>
@@ -11419,9 +12575,15 @@
         <v>3.06</v>
       </c>
       <c r="Q193" t="n">
+        <v>3515.67870000002</v>
+      </c>
+      <c r="R193" t="n">
+        <v>4558.90745226542</v>
+      </c>
+      <c r="S193" t="n">
         <v>-22.94</v>
       </c>
-      <c r="R193" t="n">
+      <c r="T193" t="n">
         <v>-23.94</v>
       </c>
     </row>
@@ -11477,9 +12639,15 @@
         <v>3.06</v>
       </c>
       <c r="Q194" t="n">
+        <v>3515.67870000002</v>
+      </c>
+      <c r="R194" t="n">
+        <v>4558.90745226542</v>
+      </c>
+      <c r="S194" t="n">
         <v>-24.84</v>
       </c>
-      <c r="R194" t="n">
+      <c r="T194" t="n">
         <v>-27.14</v>
       </c>
     </row>
@@ -11535,9 +12703,15 @@
         <v>3.06</v>
       </c>
       <c r="Q195" t="n">
+        <v>3515.67870000002</v>
+      </c>
+      <c r="R195" t="n">
+        <v>4558.90745226542</v>
+      </c>
+      <c r="S195" t="n">
         <v>-31.44</v>
       </c>
-      <c r="R195" t="n">
+      <c r="T195" t="n">
         <v>-34.34</v>
       </c>
     </row>
@@ -11593,9 +12767,15 @@
         <v>3.06</v>
       </c>
       <c r="Q196" t="n">
+        <v>3515.67870000002</v>
+      </c>
+      <c r="R196" t="n">
+        <v>4558.90745226542</v>
+      </c>
+      <c r="S196" t="n">
         <v>-38.04</v>
       </c>
-      <c r="R196" t="n">
+      <c r="T196" t="n">
         <v>-38.94</v>
       </c>
     </row>
@@ -11652,9 +12832,15 @@
         <v>-2.116</v>
       </c>
       <c r="Q197" t="n">
+        <v>9170.41893449999</v>
+      </c>
+      <c r="R197" t="n">
+        <v>3738.9778229321</v>
+      </c>
+      <c r="S197" t="n">
         <v>-32.816</v>
       </c>
-      <c r="R197" t="n">
+      <c r="T197" t="n">
         <v>-34.916</v>
       </c>
     </row>
@@ -11711,9 +12897,15 @@
         <v>-2.116</v>
       </c>
       <c r="Q198" t="n">
+        <v>9170.41893449999</v>
+      </c>
+      <c r="R198" t="n">
+        <v>3738.9778229321</v>
+      </c>
+      <c r="S198" t="n">
         <v>-34.916</v>
       </c>
-      <c r="R198" t="n">
+      <c r="T198" t="n">
         <v>-36.166</v>
       </c>
     </row>
@@ -11770,9 +12962,15 @@
         <v>-2.116</v>
       </c>
       <c r="Q199" t="n">
+        <v>9170.41893449999</v>
+      </c>
+      <c r="R199" t="n">
+        <v>3738.9778229321</v>
+      </c>
+      <c r="S199" t="n">
         <v>-40.116</v>
       </c>
-      <c r="R199" t="n">
+      <c r="T199" t="n">
         <v>-42.316</v>
       </c>
     </row>
@@ -11829,9 +13027,15 @@
         <v>-2.116</v>
       </c>
       <c r="Q200" t="n">
+        <v>9170.41893449999</v>
+      </c>
+      <c r="R200" t="n">
+        <v>3738.9778229321</v>
+      </c>
+      <c r="S200" t="n">
         <v>-42.316</v>
       </c>
-      <c r="R200" t="n">
+      <c r="T200" t="n">
         <v>-46.316</v>
       </c>
     </row>
@@ -11888,9 +13092,15 @@
         <v>-2.896</v>
       </c>
       <c r="Q201" t="n">
+        <v>7015.87897649998</v>
+      </c>
+      <c r="R201" t="n">
+        <v>3479.78898826552</v>
+      </c>
+      <c r="S201" t="n">
         <v>-18.896</v>
       </c>
-      <c r="R201" t="n">
+      <c r="T201" t="n">
         <v>-20.446</v>
       </c>
     </row>
@@ -11947,9 +13157,15 @@
         <v>-2.896</v>
       </c>
       <c r="Q202" t="n">
+        <v>7015.87897649998</v>
+      </c>
+      <c r="R202" t="n">
+        <v>3479.78898826552</v>
+      </c>
+      <c r="S202" t="n">
         <v>-20.446</v>
       </c>
-      <c r="R202" t="n">
+      <c r="T202" t="n">
         <v>-22.446</v>
       </c>
     </row>
@@ -12006,9 +13222,15 @@
         <v>-2.896</v>
       </c>
       <c r="Q203" t="n">
+        <v>7015.87897649998</v>
+      </c>
+      <c r="R203" t="n">
+        <v>3479.78898826552</v>
+      </c>
+      <c r="S203" t="n">
         <v>-22.446</v>
       </c>
-      <c r="R203" t="n">
+      <c r="T203" t="n">
         <v>-24.696</v>
       </c>
     </row>
@@ -12065,9 +13287,15 @@
         <v>-2.896</v>
       </c>
       <c r="Q204" t="n">
+        <v>7015.87897649998</v>
+      </c>
+      <c r="R204" t="n">
+        <v>3479.78898826552</v>
+      </c>
+      <c r="S204" t="n">
         <v>-24.696</v>
       </c>
-      <c r="R204" t="n">
+      <c r="T204" t="n">
         <v>-27.696</v>
       </c>
     </row>
@@ -12119,9 +13347,15 @@
         <v>4.59</v>
       </c>
       <c r="Q205" t="n">
+        <v>4528.43369999999</v>
+      </c>
+      <c r="R205" t="n">
+        <v>3275.40211893215</v>
+      </c>
+      <c r="S205" t="n">
         <v>-24.41</v>
       </c>
-      <c r="R205" t="n">
+      <c r="T205" t="n">
         <v>-25.21</v>
       </c>
     </row>
@@ -12173,9 +13407,15 @@
         <v>4.59</v>
       </c>
       <c r="Q206" t="n">
+        <v>4528.43369999999</v>
+      </c>
+      <c r="R206" t="n">
+        <v>3275.40211893215</v>
+      </c>
+      <c r="S206" t="n">
         <v>-26.41</v>
       </c>
-      <c r="R206" t="n">
+      <c r="T206" t="n">
         <v>-27.31</v>
       </c>
     </row>
@@ -12231,9 +13471,15 @@
         <v>4.59</v>
       </c>
       <c r="Q207" t="n">
+        <v>4528.43369999999</v>
+      </c>
+      <c r="R207" t="n">
+        <v>3275.40211893215</v>
+      </c>
+      <c r="S207" t="n">
         <v>-27.31</v>
       </c>
-      <c r="R207" t="n">
+      <c r="T207" t="n">
         <v>-34.91</v>
       </c>
     </row>
@@ -12289,9 +13535,15 @@
         <v>1.11</v>
       </c>
       <c r="Q208" t="n">
+        <v>1523.77770000001</v>
+      </c>
+      <c r="R208" t="n">
+        <v>1893.53678559884</v>
+      </c>
+      <c r="S208" t="n">
         <v>-17.19</v>
       </c>
-      <c r="R208" t="n">
+      <c r="T208" t="n">
         <v>-32.99</v>
       </c>
     </row>
@@ -12347,9 +13599,15 @@
         <v>0.17</v>
       </c>
       <c r="Q209" t="n">
+        <v>246.968699999998</v>
+      </c>
+      <c r="R209" t="n">
+        <v>1000.11545226537</v>
+      </c>
+      <c r="S209" t="n">
         <v>-27.23</v>
       </c>
-      <c r="R209" t="n">
+      <c r="T209" t="n">
         <v>-28.43</v>
       </c>
     </row>
@@ -12405,9 +13663,15 @@
         <v>3.22</v>
       </c>
       <c r="Q210" t="n">
+        <v>437.461199999991</v>
+      </c>
+      <c r="R210" t="n">
+        <v>-3575.27788106787</v>
+      </c>
+      <c r="S210" t="n">
         <v>-20.88</v>
       </c>
-      <c r="R210" t="n">
+      <c r="T210" t="n">
         <v>-25.68</v>
       </c>
     </row>
@@ -12463,9 +13727,15 @@
         <v>2</v>
       </c>
       <c r="Q211" t="n">
+        <v>11421.3447</v>
+      </c>
+      <c r="R211" t="n">
+        <v>-5334.00188106795</v>
+      </c>
+      <c r="S211" t="n">
         <v>-21.6</v>
       </c>
-      <c r="R211" t="n">
+      <c r="T211" t="n">
         <v>-22.25</v>
       </c>
     </row>
@@ -12521,9 +13791,15 @@
         <v>2</v>
       </c>
       <c r="Q212" t="n">
+        <v>11421.3447</v>
+      </c>
+      <c r="R212" t="n">
+        <v>-5334.00188106795</v>
+      </c>
+      <c r="S212" t="n">
         <v>-27.15</v>
       </c>
-      <c r="R212" t="n">
+      <c r="T212" t="n">
         <v>-30.1</v>
       </c>
     </row>
@@ -12579,9 +13855,15 @@
         <v>2</v>
       </c>
       <c r="Q213" t="n">
+        <v>11421.3447</v>
+      </c>
+      <c r="R213" t="n">
+        <v>-5334.00188106795</v>
+      </c>
+      <c r="S213" t="n">
         <v>-31.05</v>
       </c>
-      <c r="R213" t="n">
+      <c r="T213" t="n">
         <v>-31.6</v>
       </c>
     </row>
@@ -12637,9 +13919,15 @@
         <v>3.06</v>
       </c>
       <c r="Q214" t="n">
+        <v>8675.24370000005</v>
+      </c>
+      <c r="R214" t="n">
+        <v>-5510.93121440119</v>
+      </c>
+      <c r="S214" t="n">
         <v>-17.94</v>
       </c>
-      <c r="R214" t="n">
+      <c r="T214" t="n">
         <v>-18.64</v>
       </c>
     </row>
@@ -12695,9 +13983,15 @@
         <v>2</v>
       </c>
       <c r="Q215" t="n">
+        <v>-3185.85929999995</v>
+      </c>
+      <c r="R215" t="n">
+        <v>-5782.47388106802</v>
+      </c>
+      <c r="S215" t="n">
         <v>-15</v>
       </c>
-      <c r="R215" t="n">
+      <c r="T215" t="n">
         <v>-16.1</v>
       </c>
     </row>
@@ -12753,9 +14047,15 @@
         <v>2</v>
       </c>
       <c r="Q216" t="n">
+        <v>-3185.85929999995</v>
+      </c>
+      <c r="R216" t="n">
+        <v>-5782.47388106802</v>
+      </c>
+      <c r="S216" t="n">
         <v>-16.9</v>
       </c>
-      <c r="R216" t="n">
+      <c r="T216" t="n">
         <v>-19.3</v>
       </c>
     </row>
@@ -12811,9 +14111,15 @@
         <v>4.466</v>
       </c>
       <c r="Q217" t="n">
+        <v>-3113.64180000001</v>
+      </c>
+      <c r="R217" t="n">
+        <v>-7001.13921440113</v>
+      </c>
+      <c r="S217" t="n">
         <v>-15.534</v>
       </c>
-      <c r="R217" t="n">
+      <c r="T217" t="n">
         <v>-17.534</v>
       </c>
     </row>
@@ -12869,9 +14175,15 @@
         <v>4.466</v>
       </c>
       <c r="Q218" t="n">
+        <v>-3113.64180000001</v>
+      </c>
+      <c r="R218" t="n">
+        <v>-7001.13921440113</v>
+      </c>
+      <c r="S218" t="n">
         <v>-20.334</v>
       </c>
-      <c r="R218" t="n">
+      <c r="T218" t="n">
         <v>-21.034</v>
       </c>
     </row>
@@ -12927,9 +14239,15 @@
         <v>3.5</v>
       </c>
       <c r="Q219" t="n">
+        <v>3732.8052</v>
+      </c>
+      <c r="R219" t="n">
+        <v>4788.45078559872</v>
+      </c>
+      <c r="S219" t="n">
         <v>-18.3</v>
       </c>
-      <c r="R219" t="n">
+      <c r="T219" t="n">
         <v>-19.3</v>
       </c>
     </row>
@@ -12981,9 +14299,15 @@
         <v>3.5</v>
       </c>
       <c r="Q220" t="n">
+        <v>3732.8052</v>
+      </c>
+      <c r="R220" t="n">
+        <v>4788.45078559872</v>
+      </c>
+      <c r="S220" t="n">
         <v>-19.3</v>
       </c>
-      <c r="R220" t="n">
+      <c r="T220" t="n">
         <v>-20.4</v>
       </c>
     </row>
@@ -13039,9 +14363,15 @@
         <v>3.5</v>
       </c>
       <c r="Q221" t="n">
+        <v>3732.8052</v>
+      </c>
+      <c r="R221" t="n">
+        <v>4788.45078559872</v>
+      </c>
+      <c r="S221" t="n">
         <v>-20.4</v>
       </c>
-      <c r="R221" t="n">
+      <c r="T221" t="n">
         <v>-25.3</v>
       </c>
     </row>
@@ -13097,9 +14427,15 @@
         <v>3.5</v>
       </c>
       <c r="Q222" t="n">
+        <v>3732.8052</v>
+      </c>
+      <c r="R222" t="n">
+        <v>4788.45078559872</v>
+      </c>
+      <c r="S222" t="n">
         <v>-25.3</v>
       </c>
-      <c r="R222" t="n">
+      <c r="T222" t="n">
         <v>-26.7</v>
       </c>
     </row>
@@ -13155,9 +14491,15 @@
         <v>3.5</v>
       </c>
       <c r="Q223" t="n">
+        <v>3732.8052</v>
+      </c>
+      <c r="R223" t="n">
+        <v>4788.45078559872</v>
+      </c>
+      <c r="S223" t="n">
         <v>-31.3</v>
       </c>
-      <c r="R223" t="n">
+      <c r="T223" t="n">
         <v>-36.40000000000001</v>
       </c>
     </row>
@@ -13213,9 +14555,15 @@
         <v>3.5</v>
       </c>
       <c r="Q224" t="n">
+        <v>3732.8052</v>
+      </c>
+      <c r="R224" t="n">
+        <v>4788.45078559872</v>
+      </c>
+      <c r="S224" t="n">
         <v>-36.40000000000001</v>
       </c>
-      <c r="R224" t="n">
+      <c r="T224" t="n">
         <v>-37.90000000000001</v>
       </c>
     </row>
@@ -13271,9 +14619,15 @@
         <v>0</v>
       </c>
       <c r="Q225" t="n">
+        <v>-542.581499999942</v>
+      </c>
+      <c r="R225" t="n">
+        <v>-6104.1065477347</v>
+      </c>
+      <c r="S225" t="n">
         <v>-18.4</v>
       </c>
-      <c r="R225" t="n">
+      <c r="T225" t="n">
         <v>-25</v>
       </c>
     </row>
@@ -13329,9 +14683,15 @@
         <v>-0.26</v>
       </c>
       <c r="Q226" t="n">
+        <v>6683.12066400005</v>
+      </c>
+      <c r="R226" t="n">
+        <v>-2733.80371506792</v>
+      </c>
+      <c r="S226" t="n">
         <v>-23.26</v>
       </c>
-      <c r="R226" t="n">
+      <c r="T226" t="n">
         <v>-26.26</v>
       </c>
     </row>
@@ -13387,9 +14747,15 @@
         <v>-0.26</v>
       </c>
       <c r="Q227" t="n">
+        <v>6683.12066400005</v>
+      </c>
+      <c r="R227" t="n">
+        <v>-2733.80371506792</v>
+      </c>
+      <c r="S227" t="n">
         <v>-26.26</v>
       </c>
-      <c r="R227" t="n">
+      <c r="T227" t="n">
         <v>-27.46</v>
       </c>
     </row>
@@ -13445,9 +14811,15 @@
         <v>-0.26</v>
       </c>
       <c r="Q228" t="n">
+        <v>6683.12066400005</v>
+      </c>
+      <c r="R228" t="n">
+        <v>-2733.80371506792</v>
+      </c>
+      <c r="S228" t="n">
         <v>-27.46</v>
       </c>
-      <c r="R228" t="n">
+      <c r="T228" t="n">
         <v>-28.06</v>
       </c>
     </row>
@@ -13503,9 +14875,15 @@
         <v>-0.26</v>
       </c>
       <c r="Q229" t="n">
+        <v>6683.12066400005</v>
+      </c>
+      <c r="R229" t="n">
+        <v>-2733.80371506792</v>
+      </c>
+      <c r="S229" t="n">
         <v>-29.46</v>
       </c>
-      <c r="R229" t="n">
+      <c r="T229" t="n">
         <v>-32.06</v>
       </c>
     </row>
@@ -13561,9 +14939,15 @@
         <v>2</v>
       </c>
       <c r="Q230" t="n">
+        <v>-17063.5923</v>
+      </c>
+      <c r="R230" t="n">
+        <v>832.394785598852</v>
+      </c>
+      <c r="S230" t="n">
         <v>-20.5</v>
       </c>
-      <c r="R230" t="n">
+      <c r="T230" t="n">
         <v>-22</v>
       </c>
     </row>
@@ -13619,9 +15003,15 @@
         <v>2</v>
       </c>
       <c r="Q231" t="n">
+        <v>-17063.5923</v>
+      </c>
+      <c r="R231" t="n">
+        <v>832.394785598852</v>
+      </c>
+      <c r="S231" t="n">
         <v>-22</v>
       </c>
-      <c r="R231" t="n">
+      <c r="T231" t="n">
         <v>-24.2</v>
       </c>
     </row>
@@ -13677,9 +15067,15 @@
         <v>1</v>
       </c>
       <c r="Q232" t="n">
+        <v>-3847.13279999993</v>
+      </c>
+      <c r="R232" t="n">
+        <v>5664.91611893227</v>
+      </c>
+      <c r="S232" t="n">
         <v>-40.55</v>
       </c>
-      <c r="R232" t="n">
+      <c r="T232" t="n">
         <v>-45.34</v>
       </c>
     </row>
@@ -13735,9 +15131,15 @@
         <v>1</v>
       </c>
       <c r="Q233" t="n">
+        <v>-3847.13279999993</v>
+      </c>
+      <c r="R233" t="n">
+        <v>5664.91611893227</v>
+      </c>
+      <c r="S233" t="n">
         <v>-45.34</v>
       </c>
-      <c r="R233" t="n">
+      <c r="T233" t="n">
         <v>-48.1</v>
       </c>
     </row>
@@ -13793,9 +15195,15 @@
         <v>2.8</v>
       </c>
       <c r="Q234" t="n">
+        <v>-1650.64679999999</v>
+      </c>
+      <c r="R234" t="n">
+        <v>1347.10411893204</v>
+      </c>
+      <c r="S234" t="n">
         <v>-17.6</v>
       </c>
-      <c r="R234" t="n">
+      <c r="T234" t="n">
         <v>-27.8</v>
       </c>
     </row>

</xml_diff>